<commit_message>
adding 1st attempt at a Tableau sheet
</commit_message>
<xml_diff>
--- a/FWIP data analysis.xlsx
+++ b/FWIP data analysis.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauli\Module_20\FWIP_Venture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07F6C114-5144-4897-9982-A3E9F754FAD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EF3002-2927-4045-AE35-953BAB4498ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-435" windowWidth="29040" windowHeight="15840" xr2:uid="{D04E4B42-5AAC-4C32-AC22-35893611E54E}"/>
+    <workbookView xWindow="-57720" yWindow="-435" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D04E4B42-5AAC-4C32-AC22-35893611E54E}"/>
   </bookViews>
   <sheets>
     <sheet name="all raw data" sheetId="1" r:id="rId1"/>
-    <sheet name="Condensed" sheetId="2" r:id="rId2"/>
+    <sheet name="cleaned" sheetId="3" r:id="rId2"/>
+    <sheet name="Condensed" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="213">
   <si>
     <t>Obects</t>
   </si>
@@ -444,9 +445,6 @@
     <t>boolean</t>
   </si>
   <si>
-    <t>no idea</t>
-  </si>
-  <si>
     <t>people</t>
   </si>
   <si>
@@ -673,6 +671,9 @@
   </si>
   <si>
     <t>cash, etc</t>
+  </si>
+  <si>
+    <t>career path</t>
   </si>
 </sst>
 </file>
@@ -696,7 +697,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -718,6 +719,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,7 +782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -783,6 +790,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1099,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5017CFC6-D7F3-4668-9FDA-D7C2CD1FA3F3}">
   <dimension ref="A1:AN55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,7 +1754,7 @@
         <v>135</v>
       </c>
       <c r="H26" t="s">
-        <v>136</v>
+        <v>212</v>
       </c>
       <c r="I26" t="s">
         <v>134</v>
@@ -1754,10 +1763,10 @@
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>116</v>
@@ -1771,16 +1780,16 @@
         <v>85</v>
       </c>
       <c r="C31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" t="s">
         <v>139</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>140</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>141</v>
-      </c>
-      <c r="F31" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1791,33 +1800,33 @@
         <v>133</v>
       </c>
       <c r="C32" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" t="s">
         <v>139</v>
       </c>
-      <c r="D32" t="s">
-        <v>140</v>
-      </c>
       <c r="E32" t="s">
+        <v>142</v>
+      </c>
+      <c r="F32" t="s">
         <v>143</v>
-      </c>
-      <c r="F32" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
+        <v>158</v>
+      </c>
+      <c r="C35" t="s">
         <v>159</v>
-      </c>
-      <c r="C35" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -1828,7 +1837,7 @@
         <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
         <v>19</v>
@@ -1837,16 +1846,16 @@
         <v>25</v>
       </c>
       <c r="F36" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" t="s">
         <v>148</v>
-      </c>
-      <c r="G36" t="s">
-        <v>149</v>
       </c>
       <c r="H36" t="s">
         <v>24</v>
       </c>
       <c r="I36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J36" t="s">
         <v>23</v>
@@ -1855,10 +1864,10 @@
         <v>22</v>
       </c>
       <c r="L36" t="s">
+        <v>150</v>
+      </c>
+      <c r="M36" t="s">
         <v>151</v>
-      </c>
-      <c r="M36" t="s">
-        <v>152</v>
       </c>
       <c r="N36" t="s">
         <v>39</v>
@@ -1878,57 +1887,57 @@
         <v>90</v>
       </c>
       <c r="D37" t="s">
+        <v>152</v>
+      </c>
+      <c r="E37" t="s">
         <v>153</v>
       </c>
-      <c r="E37" t="s">
-        <v>154</v>
-      </c>
       <c r="F37" t="s">
+        <v>147</v>
+      </c>
+      <c r="G37" t="s">
         <v>148</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
+        <v>155</v>
+      </c>
+      <c r="I37" t="s">
         <v>149</v>
-      </c>
-      <c r="H37" t="s">
-        <v>156</v>
-      </c>
-      <c r="I37" t="s">
-        <v>150</v>
       </c>
       <c r="J37" t="s">
         <v>23</v>
       </c>
       <c r="K37" t="s">
+        <v>156</v>
+      </c>
+      <c r="L37" t="s">
+        <v>150</v>
+      </c>
+      <c r="M37" t="s">
+        <v>151</v>
+      </c>
+      <c r="N37" t="s">
         <v>157</v>
       </c>
-      <c r="L37" t="s">
-        <v>151</v>
-      </c>
-      <c r="M37" t="s">
-        <v>152</v>
-      </c>
-      <c r="N37" t="s">
-        <v>158</v>
-      </c>
       <c r="O37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>162</v>
-      </c>
       <c r="C40" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -1939,16 +1948,16 @@
         <v>85</v>
       </c>
       <c r="C41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" t="s">
         <v>163</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>164</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>165</v>
-      </c>
-      <c r="F41" t="s">
-        <v>166</v>
       </c>
       <c r="G41" t="s">
         <v>39</v>
@@ -1965,13 +1974,13 @@
         <v>133</v>
       </c>
       <c r="C42" t="s">
+        <v>167</v>
+      </c>
+      <c r="D42" t="s">
         <v>168</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>169</v>
-      </c>
-      <c r="E42" t="s">
-        <v>170</v>
       </c>
       <c r="F42" t="s">
         <v>81</v>
@@ -1986,10 +1995,10 @@
     <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>123</v>
@@ -2000,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C46" t="s">
         <v>85</v>
@@ -2009,7 +2018,7 @@
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F46" t="s">
         <v>101</v>
@@ -2038,25 +2047,25 @@
         <v>90</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D47" t="s">
         <v>175</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" t="s">
         <v>176</v>
       </c>
-      <c r="E47" t="s">
-        <v>81</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>177</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>178</v>
       </c>
-      <c r="H47" t="s">
+      <c r="I47" t="s">
         <v>179</v>
-      </c>
-      <c r="I47" t="s">
-        <v>180</v>
       </c>
       <c r="J47" t="s">
         <v>81</v>
@@ -2071,10 +2080,10 @@
         <v>32</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
@@ -2088,16 +2097,16 @@
         <v>85</v>
       </c>
       <c r="D50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E50" t="s">
+        <v>182</v>
+      </c>
+      <c r="F50" t="s">
         <v>183</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>184</v>
-      </c>
-      <c r="G50" t="s">
-        <v>185</v>
       </c>
       <c r="H50" t="s">
         <v>101</v>
@@ -2106,31 +2115,31 @@
         <v>102</v>
       </c>
       <c r="J50" t="s">
+        <v>185</v>
+      </c>
+      <c r="K50" t="s">
         <v>186</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>187</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>188</v>
       </c>
-      <c r="M50" t="s">
+      <c r="N50" t="s">
         <v>189</v>
       </c>
-      <c r="N50" t="s">
+      <c r="O50" t="s">
         <v>190</v>
       </c>
-      <c r="O50" t="s">
+      <c r="P50" t="s">
         <v>191</v>
       </c>
-      <c r="P50" t="s">
+      <c r="Q50" t="s">
         <v>192</v>
       </c>
-      <c r="Q50" t="s">
+      <c r="R50" t="s">
         <v>193</v>
-      </c>
-      <c r="R50" t="s">
-        <v>194</v>
       </c>
       <c r="S50" t="s">
         <v>88</v>
@@ -2165,37 +2174,37 @@
         <v>59</v>
       </c>
       <c r="F51" t="s">
+        <v>194</v>
+      </c>
+      <c r="G51" t="s">
         <v>195</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>196</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
+        <v>177</v>
+      </c>
+      <c r="J51" t="s">
+        <v>142</v>
+      </c>
+      <c r="K51" t="s">
+        <v>142</v>
+      </c>
+      <c r="L51" t="s">
+        <v>177</v>
+      </c>
+      <c r="M51" t="s">
+        <v>142</v>
+      </c>
+      <c r="N51" t="s">
+        <v>142</v>
+      </c>
+      <c r="O51" t="s">
+        <v>177</v>
+      </c>
+      <c r="P51" t="s">
         <v>197</v>
-      </c>
-      <c r="I51" t="s">
-        <v>178</v>
-      </c>
-      <c r="J51" t="s">
-        <v>143</v>
-      </c>
-      <c r="K51" t="s">
-        <v>143</v>
-      </c>
-      <c r="L51" t="s">
-        <v>178</v>
-      </c>
-      <c r="M51" t="s">
-        <v>143</v>
-      </c>
-      <c r="N51" t="s">
-        <v>143</v>
-      </c>
-      <c r="O51" t="s">
-        <v>178</v>
-      </c>
-      <c r="P51" t="s">
-        <v>198</v>
       </c>
       <c r="Q51" t="s">
         <v>135</v>
@@ -2204,13 +2213,13 @@
         <v>135</v>
       </c>
       <c r="S51" t="s">
+        <v>198</v>
+      </c>
+      <c r="T51" t="s">
         <v>199</v>
       </c>
-      <c r="T51" t="s">
+      <c r="U51" t="s">
         <v>200</v>
-      </c>
-      <c r="U51" t="s">
-        <v>201</v>
       </c>
       <c r="V51" t="s">
         <v>81</v>
@@ -2222,13 +2231,13 @@
     <row r="52" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
@@ -2236,25 +2245,25 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
+        <v>202</v>
+      </c>
+      <c r="C54" t="s">
         <v>203</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>204</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>205</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>206</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>207</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>208</v>
-      </c>
-      <c r="H54" t="s">
-        <v>209</v>
       </c>
       <c r="I54" t="s">
         <v>88</v>
@@ -2283,22 +2292,22 @@
         <v>41</v>
       </c>
       <c r="E55" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H55" t="s">
         <v>81</v>
       </c>
       <c r="I55" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K55" t="s">
         <v>81</v>
@@ -2308,17 +2317,1231 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA72ECC-5854-4FE1-97D7-D0D708886F48}">
+  <dimension ref="A1:AN56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55:J56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" t="s">
+        <v>23</v>
+      </c>
+      <c r="X2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN3" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" t="s">
+        <v>104</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" t="s">
+        <v>111</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" t="s">
+        <v>129</v>
+      </c>
+      <c r="H28" t="s">
+        <v>130</v>
+      </c>
+      <c r="I28" t="s">
+        <v>131</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" t="s">
+        <v>135</v>
+      </c>
+      <c r="H29" t="s">
+        <v>212</v>
+      </c>
+      <c r="I29" t="s">
+        <v>134</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" t="s">
+        <v>158</v>
+      </c>
+      <c r="C37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38" t="s">
+        <v>148</v>
+      </c>
+      <c r="H38" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" t="s">
+        <v>149</v>
+      </c>
+      <c r="J38" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" t="s">
+        <v>22</v>
+      </c>
+      <c r="L38" t="s">
+        <v>150</v>
+      </c>
+      <c r="M38" t="s">
+        <v>151</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" t="s">
+        <v>153</v>
+      </c>
+      <c r="F39" t="s">
+        <v>147</v>
+      </c>
+      <c r="G39" t="s">
+        <v>148</v>
+      </c>
+      <c r="H39" t="s">
+        <v>155</v>
+      </c>
+      <c r="I39" t="s">
+        <v>149</v>
+      </c>
+      <c r="J39" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" t="s">
+        <v>156</v>
+      </c>
+      <c r="L39" t="s">
+        <v>150</v>
+      </c>
+      <c r="M39" t="s">
+        <v>151</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" t="s">
+        <v>164</v>
+      </c>
+      <c r="F43" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" t="s">
+        <v>168</v>
+      </c>
+      <c r="E44" t="s">
+        <v>169</v>
+      </c>
+      <c r="F44" t="s">
+        <v>81</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>172</v>
+      </c>
+      <c r="F47" t="s">
+        <v>101</v>
+      </c>
+      <c r="G47" t="s">
+        <v>102</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D48" t="s">
+        <v>175</v>
+      </c>
+      <c r="E48" t="s">
+        <v>81</v>
+      </c>
+      <c r="F48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G48" t="s">
+        <v>177</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" t="s">
+        <v>172</v>
+      </c>
+      <c r="E51" t="s">
+        <v>182</v>
+      </c>
+      <c r="F51" t="s">
+        <v>183</v>
+      </c>
+      <c r="G51" t="s">
+        <v>184</v>
+      </c>
+      <c r="H51" t="s">
+        <v>101</v>
+      </c>
+      <c r="I51" t="s">
+        <v>102</v>
+      </c>
+      <c r="J51" t="s">
+        <v>185</v>
+      </c>
+      <c r="K51" t="s">
+        <v>186</v>
+      </c>
+      <c r="L51" t="s">
+        <v>187</v>
+      </c>
+      <c r="M51" t="s">
+        <v>188</v>
+      </c>
+      <c r="N51" t="s">
+        <v>189</v>
+      </c>
+      <c r="O51" t="s">
+        <v>190</v>
+      </c>
+      <c r="P51" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>192</v>
+      </c>
+      <c r="R51" t="s">
+        <v>193</v>
+      </c>
+      <c r="S51" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="T51" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="U51" t="s">
+        <v>38</v>
+      </c>
+      <c r="V51" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="W51" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" t="s">
+        <v>81</v>
+      </c>
+      <c r="E52" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" t="s">
+        <v>194</v>
+      </c>
+      <c r="G52" t="s">
+        <v>195</v>
+      </c>
+      <c r="H52" t="s">
+        <v>196</v>
+      </c>
+      <c r="I52" t="s">
+        <v>177</v>
+      </c>
+      <c r="J52" t="s">
+        <v>142</v>
+      </c>
+      <c r="K52" t="s">
+        <v>142</v>
+      </c>
+      <c r="L52" t="s">
+        <v>177</v>
+      </c>
+      <c r="M52" t="s">
+        <v>142</v>
+      </c>
+      <c r="N52" t="s">
+        <v>142</v>
+      </c>
+      <c r="O52" t="s">
+        <v>177</v>
+      </c>
+      <c r="P52" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>135</v>
+      </c>
+      <c r="R52" t="s">
+        <v>135</v>
+      </c>
+      <c r="S52" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="T52" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="U52" t="s">
+        <v>200</v>
+      </c>
+      <c r="V52" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="W52" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C55" t="s">
+        <v>203</v>
+      </c>
+      <c r="D55" t="s">
+        <v>204</v>
+      </c>
+      <c r="E55" t="s">
+        <v>205</v>
+      </c>
+      <c r="F55" t="s">
+        <v>206</v>
+      </c>
+      <c r="G55" t="s">
+        <v>207</v>
+      </c>
+      <c r="H55" t="s">
+        <v>208</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56" t="s">
+        <v>211</v>
+      </c>
+      <c r="F56" t="s">
+        <v>195</v>
+      </c>
+      <c r="G56" t="s">
+        <v>177</v>
+      </c>
+      <c r="H56" t="s">
+        <v>81</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1F68A3-DBCE-42B9-9D8D-76F446447055}">
   <dimension ref="A1:AG55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1:AJ1048576"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2837,6 +4060,9 @@
       <c r="G25" t="s">
         <v>129</v>
       </c>
+      <c r="H25" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -2860,14 +4086,17 @@
       <c r="G26" t="s">
         <v>135</v>
       </c>
+      <c r="H26" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
         <v>137</v>
-      </c>
-      <c r="B30" t="s">
-        <v>138</v>
       </c>
       <c r="C30" t="s">
         <v>116</v>
@@ -2881,10 +4110,10 @@
         <v>85</v>
       </c>
       <c r="C31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" t="s">
         <v>139</v>
-      </c>
-      <c r="D31" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2895,22 +4124,22 @@
         <v>133</v>
       </c>
       <c r="C32" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" t="s">
         <v>139</v>
-      </c>
-      <c r="D32" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
+        <v>158</v>
+      </c>
+      <c r="C35" t="s">
         <v>159</v>
-      </c>
-      <c r="C35" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2921,7 +4150,7 @@
         <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
         <v>19</v>
@@ -2939,10 +4168,10 @@
         <v>22</v>
       </c>
       <c r="I36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J36" t="s">
         <v>151</v>
-      </c>
-      <c r="J36" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2956,42 +4185,42 @@
         <v>90</v>
       </c>
       <c r="D37" t="s">
+        <v>152</v>
+      </c>
+      <c r="E37" t="s">
         <v>153</v>
       </c>
-      <c r="E37" t="s">
-        <v>154</v>
-      </c>
       <c r="F37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G37" t="s">
         <v>23</v>
       </c>
       <c r="H37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I37" t="s">
+        <v>150</v>
+      </c>
+      <c r="J37" t="s">
         <v>151</v>
-      </c>
-      <c r="J37" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" t="s">
         <v>161</v>
       </c>
-      <c r="B40" t="s">
-        <v>162</v>
-      </c>
       <c r="C40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3002,16 +4231,16 @@
         <v>85</v>
       </c>
       <c r="C41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" t="s">
         <v>163</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>164</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>165</v>
-      </c>
-      <c r="F41" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -3022,13 +4251,13 @@
         <v>133</v>
       </c>
       <c r="C42" t="s">
+        <v>167</v>
+      </c>
+      <c r="D42" t="s">
         <v>168</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>169</v>
-      </c>
-      <c r="E42" t="s">
-        <v>170</v>
       </c>
       <c r="F42" t="s">
         <v>81</v>
@@ -3037,10 +4266,10 @@
     <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C45" t="s">
         <v>123</v>
@@ -3051,7 +4280,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C46" t="s">
         <v>85</v>
@@ -3060,7 +4289,7 @@
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F46" t="s">
         <v>101</v>
@@ -3077,19 +4306,19 @@
         <v>90</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D47" t="s">
         <v>175</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" t="s">
         <v>176</v>
       </c>
-      <c r="E47" t="s">
-        <v>81</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>177</v>
-      </c>
-      <c r="G47" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3098,10 +4327,10 @@
         <v>32</v>
       </c>
       <c r="B49" t="s">
+        <v>180</v>
+      </c>
+      <c r="C49" t="s">
         <v>181</v>
-      </c>
-      <c r="C49" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -3115,16 +4344,16 @@
         <v>85</v>
       </c>
       <c r="D50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E50" t="s">
+        <v>182</v>
+      </c>
+      <c r="F50" t="s">
         <v>183</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>184</v>
-      </c>
-      <c r="G50" t="s">
-        <v>185</v>
       </c>
       <c r="H50" t="s">
         <v>101</v>
@@ -3133,13 +4362,13 @@
         <v>102</v>
       </c>
       <c r="J50" t="s">
+        <v>191</v>
+      </c>
+      <c r="K50" t="s">
         <v>192</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>193</v>
-      </c>
-      <c r="L50" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3159,19 +4388,19 @@
         <v>59</v>
       </c>
       <c r="F51" t="s">
+        <v>194</v>
+      </c>
+      <c r="G51" t="s">
         <v>195</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>196</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
+        <v>177</v>
+      </c>
+      <c r="J51" t="s">
         <v>197</v>
-      </c>
-      <c r="I51" t="s">
-        <v>178</v>
-      </c>
-      <c r="J51" t="s">
-        <v>198</v>
       </c>
       <c r="K51" t="s">
         <v>135</v>
@@ -3183,13 +4412,13 @@
     <row r="52" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B53" t="s">
+        <v>209</v>
+      </c>
+      <c r="C53" t="s">
         <v>210</v>
-      </c>
-      <c r="C53" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3197,25 +4426,25 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
+        <v>202</v>
+      </c>
+      <c r="C54" t="s">
         <v>203</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>204</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>205</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>206</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>207</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>208</v>
-      </c>
-      <c r="H54" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3232,13 +4461,13 @@
         <v>41</v>
       </c>
       <c r="E55" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H55" t="s">
         <v>81</v>

</xml_diff>